<commit_message>
Copy Files From Source Repo (2025-02-12 19:14)
</commit_message>
<xml_diff>
--- a/ResourceFiles/Contoso Chai Tea market trends 2023.xlsx
+++ b/ResourceFiles/Contoso Chai Tea market trends 2023.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <r>
       <rPr>
@@ -46,7 +46,7 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>Date</t>
+      <t>Fecha</t>
     </r>
   </si>
   <si>
@@ -58,7 +58,7 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>Ventas totales de Chai (unidades)</t>
+      <t>Ventas totales de chai (unidades)</t>
     </r>
   </si>
   <si>
@@ -109,6 +109,28 @@
       <t>Búsquedas en línea de Chai</t>
     </r>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>4:36</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>05:17</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -117,7 +139,7 @@
   <numFmts count="1">
     <numFmt numFmtId="177" formatCode="m/d/yyyy"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -143,6 +165,12 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -415,8 +443,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F14" totalsRowShown="0" headerRowDxfId="3" tableBorderDxfId="1" headerRowBorderDxfId="2">
   <autoFilter ref="A1:F14"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Date" dataDxfId="0"/>
-    <tableColumn id="2" name="Ventas totales de Chai (unidades)"/>
+    <tableColumn id="1" name="Fecha" dataDxfId="0"/>
+    <tableColumn id="2" name="Ventas totales de chai (unidades)"/>
     <tableColumn id="3" name="Ventas de Chai artesanal (unidades)"/>
     <tableColumn id="4" name="Ventas predefinidas de Chai (unidades)"/>
     <tableColumn id="5" name="Interacción de redes sociales (visualizaciones)"/>
@@ -844,11 +872,11 @@
       <c r="C6">
         <v>499</v>
       </c>
-      <c r="D6">
-        <v>436</v>
-      </c>
-      <c r="E6">
-        <v>1705</v>
+      <c r="D6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" t="s">
+        <v>7</v>
       </c>
       <c r="F6">
         <v>2996</v>

</xml_diff>